<commit_message>
verificação de número de coluna para testes de matching
</commit_message>
<xml_diff>
--- a/files/armazenamento.xlsx
+++ b/files/armazenamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>Tamanho em Bytes</t>
   </si>
@@ -211,6 +211,21 @@
   </si>
   <si>
     <t>Volume de dados</t>
+  </si>
+  <si>
+    <t>128mb</t>
+  </si>
+  <si>
+    <t>128000kb</t>
+  </si>
+  <si>
+    <t>Mb</t>
+  </si>
+  <si>
+    <t>Kb</t>
+  </si>
+  <si>
+    <t>bytes</t>
   </si>
 </sst>
 </file>
@@ -452,7 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,9 +478,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -475,9 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -494,15 +503,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -517,37 +517,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -931,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:X29"/>
+  <dimension ref="C3:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="I6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,8 +979,9 @@
     <col min="15" max="15" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" style="1" customWidth="1"/>
-    <col min="19" max="20" width="9.140625" style="1"/>
+    <col min="18" max="18" width="22.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="1"/>
     <col min="21" max="21" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.140625" style="1" bestFit="1" customWidth="1"/>
@@ -965,21 +990,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
-      <c r="N3" s="8" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="30"/>
+      <c r="N3" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="20"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="15"/>
     </row>
     <row r="4" spans="3:24" x14ac:dyDescent="0.25">
       <c r="F4" s="3" t="s">
@@ -991,13 +1016,13 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="19">
+      <c r="O4" s="14">
         <v>365</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="P4" s="17" t="s">
         <v>32</v>
       </c>
       <c r="Q4" s="3" t="s">
@@ -1026,13 +1051,13 @@
         <v>3460</v>
       </c>
       <c r="J5" s="3"/>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="O5" s="19">
+      <c r="O5" s="14">
         <v>24</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="17" t="s">
         <v>33</v>
       </c>
       <c r="Q5" s="3" t="s">
@@ -1042,10 +1067,10 @@
         <v>8</v>
       </c>
       <c r="U5" s="2"/>
-      <c r="V5" s="18" t="s">
+      <c r="V5" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="W5" s="12">
+      <c r="W5" s="10">
         <f>R26</f>
         <v>169</v>
       </c>
@@ -1064,17 +1089,17 @@
         <f>G6*8</f>
         <v>6920</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="8">
         <f>SUM(I5:I6)</f>
         <v>10380</v>
       </c>
-      <c r="N6" s="29" t="s">
+      <c r="N6" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O6" s="29">
+      <c r="O6" s="21">
         <v>60</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="P6" s="17" t="s">
         <v>34</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -1087,7 +1112,7 @@
       <c r="V6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="W6" s="12">
+      <c r="W6" s="10">
         <v>525600</v>
       </c>
       <c r="X6" s="2"/>
@@ -1103,15 +1128,15 @@
         <f>J6*I7</f>
         <v>51900</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="N7" s="30" t="s">
+      <c r="K7" s="11"/>
+      <c r="N7" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O7" s="23">
         <f>O4*O5*O6</f>
         <v>525600</v>
       </c>
-      <c r="P7" s="23" t="s">
+      <c r="P7" s="17" t="s">
         <v>35</v>
       </c>
       <c r="Q7" s="3" t="s">
@@ -1120,7 +1145,7 @@
       <c r="R7" s="3">
         <v>8</v>
       </c>
-      <c r="W7" s="9">
+      <c r="W7" s="7">
         <f>R26*W6</f>
         <v>88826400</v>
       </c>
@@ -1135,14 +1160,14 @@
       <c r="I8" s="3">
         <v>365</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="7">
         <f>J7*I8</f>
         <v>18943500</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="17" t="s">
         <v>37</v>
       </c>
       <c r="Q8" s="3" t="s">
@@ -1162,9 +1187,9 @@
       </c>
     </row>
     <row r="9" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
       <c r="J9" s="3">
         <f>J8/1000</f>
         <v>18943.5</v>
@@ -1172,7 +1197,7 @@
       <c r="K9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="23" t="s">
+      <c r="P9" s="17" t="s">
         <v>36</v>
       </c>
       <c r="Q9" s="3" t="s">
@@ -1183,7 +1208,7 @@
       </c>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
-      <c r="W9" s="11">
+      <c r="W9" s="9">
         <f>W8/1000</f>
         <v>88.826399999999992</v>
       </c>
@@ -1192,17 +1217,17 @@
       </c>
     </row>
     <row r="10" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="J10" s="11">
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="J10" s="9">
         <f>J9/1000</f>
         <v>18.9435</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="23" t="s">
+      <c r="P10" s="17" t="s">
         <v>38</v>
       </c>
       <c r="Q10" s="3" t="s">
@@ -1213,9 +1238,9 @@
       </c>
     </row>
     <row r="11" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="P11" s="23" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="P11" s="17" t="s">
         <v>39</v>
       </c>
       <c r="Q11" s="3" t="s">
@@ -1226,9 +1251,9 @@
       </c>
     </row>
     <row r="12" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="P12" s="23" t="s">
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="P12" s="17" t="s">
         <v>40</v>
       </c>
       <c r="Q12" s="3" t="s">
@@ -1239,8 +1264,8 @@
       </c>
     </row>
     <row r="13" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="F13" s="21"/>
-      <c r="P13" s="23" t="s">
+      <c r="F13" s="16"/>
+      <c r="P13" s="17" t="s">
         <v>41</v>
       </c>
       <c r="Q13" s="3" t="s">
@@ -1251,14 +1276,14 @@
       </c>
     </row>
     <row r="14" spans="3:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P14" s="23" t="s">
+      <c r="P14" s="17" t="s">
         <v>42</v>
       </c>
       <c r="Q14" s="3" t="s">
@@ -1269,16 +1294,16 @@
       </c>
     </row>
     <row r="15" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>1</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="P15" s="23" t="s">
+      <c r="P15" s="17" t="s">
         <v>43</v>
       </c>
       <c r="Q15" s="3" t="s">
@@ -1287,22 +1312,22 @@
       <c r="R15" s="3">
         <v>8</v>
       </c>
-      <c r="W15" s="4" t="s">
+      <c r="W15" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="X15" s="4"/>
+      <c r="X15" s="27"/>
     </row>
     <row r="16" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="P16" s="23" t="s">
+      <c r="P16" s="17" t="s">
         <v>44</v>
       </c>
       <c r="Q16" s="3" t="s">
@@ -1311,24 +1336,24 @@
       <c r="R16" s="3">
         <v>8</v>
       </c>
-      <c r="W16" s="11">
+      <c r="W16" s="9">
         <v>21.9</v>
       </c>
-      <c r="X16" s="32">
+      <c r="X16" s="24">
         <v>88.30080000000001</v>
       </c>
     </row>
     <row r="17" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>1</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="P17" s="23" t="s">
+      <c r="P17" s="17" t="s">
         <v>45</v>
       </c>
       <c r="Q17" s="3" t="s">
@@ -1337,23 +1362,23 @@
       <c r="R17" s="3">
         <v>8</v>
       </c>
-      <c r="W17" s="4">
+      <c r="W17" s="27">
         <f>SUM(W16:X16)</f>
         <v>110.20080000000002</v>
       </c>
-      <c r="X17" s="4"/>
+      <c r="X17" s="27"/>
     </row>
     <row r="18" spans="3:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>4</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="P18" s="23" t="s">
+      <c r="E18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P18" s="17" t="s">
         <v>46</v>
       </c>
       <c r="Q18" s="3" t="s">
@@ -1364,16 +1389,16 @@
       </c>
     </row>
     <row r="19" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>4</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P19" s="23" t="s">
+      <c r="P19" s="17" t="s">
         <v>47</v>
       </c>
       <c r="Q19" s="3" t="s">
@@ -1384,16 +1409,16 @@
       </c>
     </row>
     <row r="20" spans="3:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>4</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="P20" s="23" t="s">
+      <c r="E20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P20" s="17" t="s">
         <v>48</v>
       </c>
       <c r="Q20" s="3" t="s">
@@ -1404,16 +1429,16 @@
       </c>
     </row>
     <row r="21" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>2</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P21" s="23" t="s">
+      <c r="P21" s="17" t="s">
         <v>49</v>
       </c>
       <c r="Q21" s="3" t="s">
@@ -1424,16 +1449,16 @@
       </c>
     </row>
     <row r="22" spans="3:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>2</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P22" s="23" t="s">
+      <c r="P22" s="17" t="s">
         <v>50</v>
       </c>
       <c r="Q22" s="3" t="s">
@@ -1444,16 +1469,16 @@
       </c>
     </row>
     <row r="23" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>2</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P23" s="23" t="s">
+      <c r="P23" s="17" t="s">
         <v>51</v>
       </c>
       <c r="Q23" s="3" t="s">
@@ -1464,16 +1489,16 @@
       </c>
     </row>
     <row r="24" spans="3:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>4</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="P24" s="23" t="s">
+      <c r="E24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24" s="17" t="s">
         <v>52</v>
       </c>
       <c r="Q24" s="3" t="s">
@@ -1484,75 +1509,131 @@
       </c>
     </row>
     <row r="25" spans="3:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>4</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="P25" s="24" t="s">
+      <c r="E25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P25" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="Q25" s="25" t="s">
+      <c r="Q25" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="R25" s="25">
+      <c r="R25" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>4</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P26" s="26" t="s">
+      <c r="P26" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="28">
+      <c r="Q26" s="26"/>
+      <c r="R26" s="20">
         <f>SUM(R4:R25)</f>
         <v>169</v>
       </c>
     </row>
     <row r="27" spans="3:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>4</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="3:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="7">
-        <v>8</v>
-      </c>
-      <c r="E28" s="7" t="s">
+      <c r="D28" s="6">
+        <v>8</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="R28" s="1">
+        <v>169</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="29" spans="3:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>10</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="6" t="s">
         <v>23</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="R30" s="1">
+        <v>169</v>
+      </c>
+      <c r="S30" s="1">
+        <v>128000000</v>
+      </c>
+    </row>
+    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="R31" s="33">
+        <f>S30/R30-1</f>
+        <v>757395.44970414205</v>
+      </c>
+    </row>
+    <row r="32" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="R32" s="1">
+        <f>O7/R31</f>
+        <v>0.693957166240321</v>
+      </c>
+    </row>
+    <row r="33" spans="18:19" x14ac:dyDescent="0.25">
+      <c r="R33" s="34">
+        <f>R32*S30</f>
+        <v>88826517.278761089</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="18:19" x14ac:dyDescent="0.25">
+      <c r="R34" s="35">
+        <f>R33/1000</f>
+        <v>88826.517278761094</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="18:19" x14ac:dyDescent="0.25">
+      <c r="R35" s="35">
+        <f>R34/1000</f>
+        <v>88.826517278761088</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>